<commit_message>
[DESC]: Updated folder name
</commit_message>
<xml_diff>
--- a/r1_test_command_list_tag1.0.xlsx
+++ b/r1_test_command_list_tag1.0.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13725"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="commands_list" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
@@ -600,7 +600,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>